<commit_message>
Added population and income to route dataset
</commit_message>
<xml_diff>
--- a/Income.xlsx
+++ b/Income.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aparma\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="20490" windowHeight="8985" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Income" sheetId="1" r:id="rId1"/>
     <sheet name="Categorization" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="65">
   <si>
     <t>Atlanta</t>
   </si>
@@ -217,6 +212,9 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Locid</t>
   </si>
 </sst>
 </file>
@@ -887,7 +885,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -922,7 +920,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1099,7 +1097,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1109,8 +1107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z32"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2299,10 +2297,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E7" sqref="B6:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2312,7 +2310,7 @@
     <col min="4" max="4" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="16" t="s">
         <v>59</v>
       </c>
@@ -2322,8 +2320,11 @@
       <c r="D1" s="16" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -2336,8 +2337,11 @@
       <c r="D2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -2350,8 +2354,11 @@
       <c r="D3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -2364,8 +2371,11 @@
       <c r="D4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>24</v>
       </c>
@@ -2378,8 +2388,11 @@
       <c r="D5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
@@ -2392,8 +2405,11 @@
       <c r="D6" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
@@ -2406,8 +2422,11 @@
       <c r="D7" s="16" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
@@ -2420,8 +2439,11 @@
       <c r="D8" s="16" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>6</v>
       </c>
@@ -2434,8 +2456,11 @@
       <c r="D9" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>7</v>
       </c>
@@ -2448,8 +2473,11 @@
       <c r="D10" s="16" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
@@ -2462,8 +2490,11 @@
       <c r="D11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
@@ -2476,8 +2507,11 @@
       <c r="D12" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>10</v>
       </c>
@@ -2490,8 +2524,11 @@
       <c r="D13" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>11</v>
       </c>
@@ -2504,8 +2541,11 @@
       <c r="D14" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>12</v>
       </c>
@@ -2518,8 +2558,11 @@
       <c r="D15" s="16" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>13</v>
       </c>
@@ -2532,8 +2575,11 @@
       <c r="D16" s="16" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>14</v>
       </c>
@@ -2546,8 +2592,11 @@
       <c r="D17" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>15</v>
       </c>
@@ -2560,8 +2609,11 @@
       <c r="D18" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>16</v>
       </c>
@@ -2574,8 +2626,11 @@
       <c r="D19" s="16" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>17</v>
       </c>
@@ -2588,8 +2643,11 @@
       <c r="D20" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>3</v>
       </c>
@@ -2602,8 +2660,11 @@
       <c r="D21" s="16" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>18</v>
       </c>
@@ -2616,8 +2677,11 @@
       <c r="D22" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="E22" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>55</v>
       </c>
@@ -2630,8 +2694,11 @@
       <c r="D23" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
         <v>56</v>
       </c>
@@ -2644,8 +2711,11 @@
       <c r="D24" s="21" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>2</v>
       </c>
@@ -2658,8 +2728,11 @@
       <c r="D25" s="16" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>19</v>
       </c>
@@ -2672,8 +2745,11 @@
       <c r="D26" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>58</v>
       </c>
@@ -2686,8 +2762,11 @@
       <c r="D27" s="21" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>20</v>
       </c>
@@ -2700,8 +2779,11 @@
       <c r="D28" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>21</v>
       </c>
@@ -2714,8 +2796,11 @@
       <c r="D29" s="16" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
         <v>22</v>
       </c>
@@ -2728,8 +2813,11 @@
       <c r="D30" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>23</v>
       </c>
@@ -2742,8 +2830,11 @@
       <c r="D31" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>